<commit_message>
1. rename UserPermissionHelper to CacheHelper
2. use CacheHelper to retrieve data from the server cache with unique user ID key before requery the database
</commit_message>
<xml_diff>
--- a/Copy of VSSC Feedback July 2 2021.xlsx
+++ b/Copy of VSSC Feedback July 2 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VHAPORSUNC\source\repos\VSSC\IPRehab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805F5F9A-C951-4977-B53B-6970E047B9A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621D89BE-5BE3-4D02-BBBE-5CCA0EBD2D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="3" activeTab="7" xr2:uid="{D57B31B5-7152-463E-ABC6-71BF39CFCF39}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{D57B31B5-7152-463E-ABC6-71BF39CFCF39}"/>
   </bookViews>
   <sheets>
     <sheet name="Treating Specialty Codes" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="82">
   <si>
     <t>Q 17 "Pre-hospital Living with"</t>
   </si>
@@ -371,6 +371,12 @@
   </si>
   <si>
     <t>in conflict with 03/20/21 worksheet where GG0130A-Discharge Goals is not included</t>
+  </si>
+  <si>
+    <t>Assessment Completed</t>
+  </si>
+  <si>
+    <t>Discharge Performance and Discharge Goal?</t>
   </si>
 </sst>
 </file>
@@ -970,7 +976,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A22" sqref="A22:XFD24"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
@@ -1326,7 +1332,7 @@
   </sheetPr>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A2:XFD3"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
@@ -1621,9 +1627,9 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A24" sqref="A24:XFD26"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1690,6 +1696,9 @@
       <c r="B8" s="21" t="s">
         <v>63</v>
       </c>
+      <c r="C8" s="22" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20"/>
@@ -1702,8 +1711,8 @@
       <c r="B10" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>79</v>
+      <c r="C10" s="23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.35">
@@ -1747,8 +1756,8 @@
       <c r="B19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>52</v>
+      <c r="C19" s="23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1778,7 +1787,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1793,7 +1802,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -1945,10 +1954,10 @@
   </sheetPr>
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C18" sqref="C18"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2075,8 +2084,8 @@
       <c r="B19" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>52</v>
+      <c r="C19" s="15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2105,6 +2114,9 @@
       <c r="B23" s="25" t="s">
         <v>46</v>
       </c>
+      <c r="C23" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
@@ -2182,6 +2194,9 @@
       </c>
       <c r="B35" s="24" t="s">
         <v>30</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>